<commit_message>
-WQC edits to fix map
</commit_message>
<xml_diff>
--- a/inputs/Stream Use Designations Herrera.xlsx
+++ b/inputs/Stream Use Designations Herrera.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://herrerainc-my.sharepoint.com/personal/nharris_herrerainc_com/Documents/Documents/Projects/4_GitHub/23-08082-000-TC-WQ-Dashboard/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00BDE8B-B78E-4727-A8E3-AD509779A97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C00BDE8B-B78E-4727-A8E3-AD509779A97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84C25CA6-05BB-414E-B9D8-7FC2A4B49762}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9870" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ThurstonCoWQData_2023-07-31" sheetId="1" r:id="rId1"/>
@@ -1029,9 +1029,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1069,7 +1069,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1175,7 +1175,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1317,7 +1317,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1327,19 +1327,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="60.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1356,7 +1357,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>41</v>
       </c>
@@ -1364,7 +1365,7 @@
       <c r="D2" s="9"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:5" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -1415,7 +1416,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1449,7 +1450,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>58</v>
       </c>
@@ -1466,7 +1467,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>60</v>
       </c>
@@ -1500,7 +1501,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>62</v>
       </c>
@@ -1534,7 +1535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>63</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
@@ -1568,7 +1569,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>66</v>
       </c>
@@ -1602,7 +1603,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>68</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -1653,7 +1654,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>71</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
@@ -1704,7 +1705,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
@@ -1721,7 +1722,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>75</v>
       </c>
@@ -1738,7 +1739,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>76</v>
       </c>
@@ -1755,7 +1756,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>77</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>78</v>
       </c>
@@ -1789,7 +1790,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>79</v>
       </c>
@@ -1806,7 +1807,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>80</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>81</v>
       </c>
@@ -1840,7 +1841,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>82</v>
       </c>
@@ -1857,7 +1858,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>83</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>84</v>
       </c>
@@ -1891,7 +1892,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>85</v>
       </c>
@@ -1908,7 +1909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>86</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>87</v>
       </c>
@@ -1942,7 +1943,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>40</v>
       </c>
@@ -1950,7 +1951,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -1967,23 +1968,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
         <v>48</v>
       </c>

</xml_diff>